<commit_message>
Project Batch 30 Dec 2023
Project Batch 30 Dec 2023
</commit_message>
<xml_diff>
--- a/Project batch Sheet/Project Batch Sheet.xlsx
+++ b/Project batch Sheet/Project Batch Sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Angular\JavaScript\Project batch Sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2C9FFED-22B3-4BBF-8CB8-4A4383CE3C55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9870C5ED-D343-44C4-8373-57783DEC905D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="735" yWindow="735" windowWidth="15375" windowHeight="7875" xr2:uid="{F43F5E3C-0558-E346-B770-8540CD6B4863}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{F43F5E3C-0558-E346-B770-8540CD6B4863}"/>
   </bookViews>
   <sheets>
     <sheet name="Dec-2023" sheetId="1" r:id="rId1"/>
@@ -24,8 +24,67 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Hp</author>
+  </authors>
+  <commentList>
+    <comment ref="D3" authorId="0" shapeId="0" xr:uid="{0A17E92C-6FF0-4A33-A645-E6D149F8902C}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Hp:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Family gate together &amp; Going to Temple</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D7" authorId="0" shapeId="0" xr:uid="{537A38CA-D15F-4AB4-A182-B03C454B3293}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Hp:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Go to the Affidavits Medical Certificate &amp; Non Creamy layer Certificate
+She not attend Lecture</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="12">
   <si>
     <t>Student Name</t>
   </si>
@@ -58,13 +117,16 @@
   </si>
   <si>
     <t>Snehal patil</t>
+  </si>
+  <si>
+    <t>Reason</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -86,6 +148,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -466,17 +541,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF336CF2-9F7E-9D47-A242-C3CB362C49F8}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF336CF2-9F7E-9D47-A242-C3CB362C49F8}">
   <dimension ref="A1:T12"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6.125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
@@ -489,7 +565,9 @@
       <c r="C1" s="4">
         <v>45289</v>
       </c>
-      <c r="D1" s="4"/>
+      <c r="D1" s="4">
+        <v>45290</v>
+      </c>
       <c r="E1" s="5"/>
       <c r="F1" s="5"/>
       <c r="G1" s="5"/>
@@ -517,7 +595,9 @@
       <c r="C2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="7"/>
+      <c r="D2" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="E2" s="7"/>
       <c r="F2" s="7"/>
       <c r="G2" s="7"/>
@@ -545,7 +625,9 @@
       <c r="C3" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="7"/>
+      <c r="D3" s="7" t="s">
+        <v>11</v>
+      </c>
       <c r="E3" s="7"/>
       <c r="F3" s="7"/>
       <c r="G3" s="7"/>
@@ -573,7 +655,9 @@
       <c r="C4" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="7"/>
+      <c r="D4" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="E4" s="7"/>
       <c r="F4" s="7"/>
       <c r="G4" s="7"/>
@@ -601,7 +685,9 @@
       <c r="C5" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="7"/>
+      <c r="D5" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="E5" s="7"/>
       <c r="F5" s="7"/>
       <c r="G5" s="7"/>
@@ -629,7 +715,9 @@
       <c r="C6" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="7"/>
+      <c r="D6" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="E6" s="7"/>
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
@@ -657,7 +745,9 @@
       <c r="C7" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D7" s="7"/>
+      <c r="D7" s="7" t="s">
+        <v>11</v>
+      </c>
       <c r="E7" s="7"/>
       <c r="F7" s="7"/>
       <c r="G7" s="7"/>
@@ -685,7 +775,9 @@
       <c r="C8" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D8" s="7"/>
+      <c r="D8" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="E8" s="7"/>
       <c r="F8" s="7"/>
       <c r="G8" s="7"/>
@@ -716,5 +808,6 @@
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Attendance on 01 Jan 2024
Attendance on 01 Jan 2024
</commit_message>
<xml_diff>
--- a/Project batch Sheet/Project Batch Sheet.xlsx
+++ b/Project batch Sheet/Project Batch Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Angular\JavaScript\Project batch Sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9870C5ED-D343-44C4-8373-57783DEC905D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A160875F-E848-4A2B-848E-8D0799BDDFB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{F43F5E3C-0558-E346-B770-8540CD6B4863}"/>
   </bookViews>
@@ -30,6 +30,30 @@
     <author>Hp</author>
   </authors>
   <commentList>
+    <comment ref="E2" authorId="0" shapeId="0" xr:uid="{DB85F54B-2016-4DCB-8ED7-68D1B5D97712}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Hp:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Family Emergency</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="D3" authorId="0" shapeId="0" xr:uid="{0A17E92C-6FF0-4A33-A645-E6D149F8902C}">
       <text>
         <r>
@@ -51,6 +75,54 @@
           </rPr>
           <t xml:space="preserve">
 Family gate together &amp; Going to Temple</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E3" authorId="0" shapeId="0" xr:uid="{F36DD893-457C-4985-BF74-37599E2DDE97}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Hp:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Out of Town</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E5" authorId="0" shapeId="0" xr:uid="{E1A6D40D-C230-4FE8-BAE1-D6B369291E94}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Hp:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Outside the Pune</t>
         </r>
       </text>
     </comment>
@@ -84,7 +156,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="12">
   <si>
     <t>Student Name</t>
   </si>
@@ -126,7 +198,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -161,6 +233,19 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -545,7 +630,7 @@
   <dimension ref="A1:T12"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -568,7 +653,9 @@
       <c r="D1" s="4">
         <v>45290</v>
       </c>
-      <c r="E1" s="5"/>
+      <c r="E1" s="4">
+        <v>45292</v>
+      </c>
       <c r="F1" s="5"/>
       <c r="G1" s="5"/>
       <c r="H1" s="5"/>
@@ -598,7 +685,9 @@
       <c r="D2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="7"/>
+      <c r="E2" s="7" t="s">
+        <v>11</v>
+      </c>
       <c r="F2" s="7"/>
       <c r="G2" s="7"/>
       <c r="H2" s="7"/>
@@ -628,7 +717,9 @@
       <c r="D3" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="7"/>
+      <c r="E3" s="7" t="s">
+        <v>11</v>
+      </c>
       <c r="F3" s="7"/>
       <c r="G3" s="7"/>
       <c r="H3" s="7"/>
@@ -658,7 +749,9 @@
       <c r="D4" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="7"/>
+      <c r="E4" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="F4" s="7"/>
       <c r="G4" s="7"/>
       <c r="H4" s="7"/>
@@ -688,7 +781,9 @@
       <c r="D5" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="E5" s="7"/>
+      <c r="E5" s="7" t="s">
+        <v>11</v>
+      </c>
       <c r="F5" s="7"/>
       <c r="G5" s="7"/>
       <c r="H5" s="7"/>
@@ -718,7 +813,9 @@
       <c r="D6" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="E6" s="7"/>
+      <c r="E6" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
       <c r="H6" s="7"/>
@@ -748,7 +845,9 @@
       <c r="D7" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="7"/>
+      <c r="E7" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="F7" s="7"/>
       <c r="G7" s="7"/>
       <c r="H7" s="7"/>
@@ -778,7 +877,9 @@
       <c r="D8" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="E8" s="7"/>
+      <c r="E8" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="F8" s="7"/>
       <c r="G8" s="7"/>
       <c r="H8" s="7"/>

</xml_diff>

<commit_message>
Team Meet Up 02 Jan 2024
Team Meet Up 02 Jan 2024
</commit_message>
<xml_diff>
--- a/Project batch Sheet/Project Batch Sheet.xlsx
+++ b/Project batch Sheet/Project Batch Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Angular\JavaScript\Project batch Sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A160875F-E848-4A2B-848E-8D0799BDDFB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D76FF0A-4631-42A5-BB86-4B5865016BF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{F43F5E3C-0558-E346-B770-8540CD6B4863}"/>
   </bookViews>
@@ -126,6 +126,30 @@
         </r>
       </text>
     </comment>
+    <comment ref="F5" authorId="0" shapeId="0" xr:uid="{D6517C62-E677-4066-97D1-77459AA107DD}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Hp:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Health Issue</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="D7" authorId="0" shapeId="0" xr:uid="{537A38CA-D15F-4AB4-A182-B03C454B3293}">
       <text>
         <r>
@@ -148,6 +172,30 @@
           <t xml:space="preserve">
 Go to the Affidavits Medical Certificate &amp; Non Creamy layer Certificate
 She not attend Lecture</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F7" authorId="0" shapeId="0" xr:uid="{4C6B5908-5B4E-4BFA-B0E6-9FB5FACD637F}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Hp:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Outside the Pune</t>
         </r>
       </text>
     </comment>
@@ -156,7 +204,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="12">
   <si>
     <t>Student Name</t>
   </si>
@@ -630,7 +678,7 @@
   <dimension ref="A1:T12"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -656,7 +704,9 @@
       <c r="E1" s="4">
         <v>45292</v>
       </c>
-      <c r="F1" s="5"/>
+      <c r="F1" s="4">
+        <v>45293</v>
+      </c>
       <c r="G1" s="5"/>
       <c r="H1" s="5"/>
       <c r="I1" s="5"/>
@@ -688,7 +738,9 @@
       <c r="E2" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="7"/>
+      <c r="F2" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="G2" s="7"/>
       <c r="H2" s="7"/>
       <c r="I2" s="7"/>
@@ -720,7 +772,9 @@
       <c r="E3" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="7"/>
+      <c r="F3" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="G3" s="7"/>
       <c r="H3" s="7"/>
       <c r="I3" s="7"/>
@@ -752,7 +806,9 @@
       <c r="E4" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="7"/>
+      <c r="F4" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="G4" s="7"/>
       <c r="H4" s="7"/>
       <c r="I4" s="7"/>
@@ -784,7 +840,9 @@
       <c r="E5" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="7"/>
+      <c r="F5" s="7" t="s">
+        <v>11</v>
+      </c>
       <c r="G5" s="7"/>
       <c r="H5" s="7"/>
       <c r="I5" s="7"/>
@@ -816,7 +874,9 @@
       <c r="E6" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="F6" s="7"/>
+      <c r="F6" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="G6" s="7"/>
       <c r="H6" s="7"/>
       <c r="I6" s="7"/>
@@ -848,7 +908,9 @@
       <c r="E7" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="F7" s="7"/>
+      <c r="F7" s="7" t="s">
+        <v>11</v>
+      </c>
       <c r="G7" s="7"/>
       <c r="H7" s="7"/>
       <c r="I7" s="7"/>
@@ -880,7 +942,9 @@
       <c r="E8" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="F8" s="7"/>
+      <c r="F8" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="G8" s="7"/>
       <c r="H8" s="7"/>
       <c r="I8" s="7"/>
@@ -903,7 +967,7 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:E8" xr:uid="{F036FACA-372A-8349-BD3D-950830E988A4}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:N8" xr:uid="{F036FACA-372A-8349-BD3D-950830E988A4}">
       <formula1>"Present, Absent,Reason"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Meeting at 03 Jan 2024
Meeting at 03 Jan 2024
</commit_message>
<xml_diff>
--- a/Project batch Sheet/Project Batch Sheet.xlsx
+++ b/Project batch Sheet/Project Batch Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Angular\JavaScript\Project batch Sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D76FF0A-4631-42A5-BB86-4B5865016BF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33661D8A-39E2-4819-AE29-8B68256E3C36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{F43F5E3C-0558-E346-B770-8540CD6B4863}"/>
   </bookViews>
@@ -204,7 +204,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="14">
   <si>
     <t>Student Name</t>
   </si>
@@ -240,6 +240,12 @@
   </si>
   <si>
     <t>Reason</t>
+  </si>
+  <si>
+    <t>Ayesha Singh</t>
+  </si>
+  <si>
+    <t>Absent</t>
   </si>
 </sst>
 </file>
@@ -707,7 +713,9 @@
       <c r="F1" s="4">
         <v>45293</v>
       </c>
-      <c r="G1" s="5"/>
+      <c r="G1" s="4">
+        <v>45294</v>
+      </c>
       <c r="H1" s="5"/>
       <c r="I1" s="5"/>
       <c r="J1" s="5"/>
@@ -741,7 +749,9 @@
       <c r="F2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="7"/>
+      <c r="G2" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="H2" s="7"/>
       <c r="I2" s="7"/>
       <c r="J2" s="7"/>
@@ -775,7 +785,9 @@
       <c r="F3" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="G3" s="7"/>
+      <c r="G3" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="H3" s="7"/>
       <c r="I3" s="7"/>
       <c r="J3" s="7"/>
@@ -809,7 +821,9 @@
       <c r="F4" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="7"/>
+      <c r="G4" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="H4" s="7"/>
       <c r="I4" s="7"/>
       <c r="J4" s="7"/>
@@ -843,7 +857,9 @@
       <c r="F5" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="G5" s="7"/>
+      <c r="G5" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="H5" s="7"/>
       <c r="I5" s="7"/>
       <c r="J5" s="7"/>
@@ -877,7 +893,9 @@
       <c r="F6" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="G6" s="7"/>
+      <c r="G6" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="H6" s="7"/>
       <c r="I6" s="7"/>
       <c r="J6" s="7"/>
@@ -911,7 +929,9 @@
       <c r="F7" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="G7" s="7"/>
+      <c r="G7" s="7" t="s">
+        <v>13</v>
+      </c>
       <c r="H7" s="7"/>
       <c r="I7" s="7"/>
       <c r="J7" s="7"/>
@@ -945,7 +965,9 @@
       <c r="F8" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="G8" s="7"/>
+      <c r="G8" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="H8" s="7"/>
       <c r="I8" s="7"/>
       <c r="J8" s="7"/>
@@ -960,6 +982,42 @@
       <c r="S8" s="7"/>
       <c r="T8" s="7"/>
     </row>
+    <row r="9" spans="1:20" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A9" s="6">
+        <v>8</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="H9" s="7"/>
+      <c r="I9" s="7"/>
+      <c r="J9" s="7"/>
+      <c r="K9" s="7"/>
+      <c r="L9" s="7"/>
+      <c r="M9" s="7"/>
+      <c r="N9" s="7"/>
+      <c r="O9" s="7"/>
+      <c r="P9" s="7"/>
+      <c r="Q9" s="7"/>
+      <c r="R9" s="7"/>
+      <c r="S9" s="7"/>
+      <c r="T9" s="7"/>
+    </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B12" s="8" t="s">
         <v>3</v>
@@ -967,7 +1025,7 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:N8" xr:uid="{F036FACA-372A-8349-BD3D-950830E988A4}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:N9" xr:uid="{F036FACA-372A-8349-BD3D-950830E988A4}">
       <formula1>"Present, Absent,Reason"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Google Meet Attendance 04 jan 2024
Google Meet Attendance 04 jan 2024
</commit_message>
<xml_diff>
--- a/Project batch Sheet/Project Batch Sheet.xlsx
+++ b/Project batch Sheet/Project Batch Sheet.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Angular\JavaScript\Project batch Sheet\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Angular\JavaScript\Project batch Sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33661D8A-39E2-4819-AE29-8B68256E3C36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CEC8294-D33B-4161-B178-1F5AD5F9BAFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{F43F5E3C-0558-E346-B770-8540CD6B4863}"/>
   </bookViews>
@@ -28,6 +28,7 @@
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Hp</author>
+    <author>Admin</author>
   </authors>
   <commentList>
     <comment ref="E2" authorId="0" shapeId="0" xr:uid="{DB85F54B-2016-4DCB-8ED7-68D1B5D97712}">
@@ -54,6 +55,22 @@
         </r>
       </text>
     </comment>
+    <comment ref="H2" authorId="1" shapeId="0" xr:uid="{CE5CDF55-7556-445E-930F-4AD485DEB387}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Admin:
+travelling in train 
+Reached late from office</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="D3" authorId="0" shapeId="0" xr:uid="{0A17E92C-6FF0-4A33-A645-E6D149F8902C}">
       <text>
         <r>
@@ -102,6 +119,30 @@
         </r>
       </text>
     </comment>
+    <comment ref="H3" authorId="1" shapeId="0" xr:uid="{A0F254C2-0AC4-4546-9DE5-0BDC870ACB26}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Admin:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Unavailable for Meet</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="E5" authorId="0" shapeId="0" xr:uid="{E1A6D40D-C230-4FE8-BAE1-D6B369291E94}">
       <text>
         <r>
@@ -196,6 +237,54 @@
           </rPr>
           <t xml:space="preserve">
 Outside the Pune</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H7" authorId="1" shapeId="0" xr:uid="{BD8EEB3F-A9D3-40C0-B664-90CEC5169992}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Admin:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Relocating the Home</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H9" authorId="1" shapeId="0" xr:uid="{878DF12F-2629-4626-9ED2-8FCBC10AFEBF}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Admin:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Travelling</t>
         </r>
       </text>
     </comment>
@@ -204,7 +293,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="14">
   <si>
     <t>Student Name</t>
   </si>
@@ -684,7 +773,7 @@
   <dimension ref="A1:T12"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="G2" sqref="D1:G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -716,7 +805,9 @@
       <c r="G1" s="4">
         <v>45294</v>
       </c>
-      <c r="H1" s="5"/>
+      <c r="H1" s="4">
+        <v>45295</v>
+      </c>
       <c r="I1" s="5"/>
       <c r="J1" s="5"/>
       <c r="K1" s="5"/>
@@ -752,7 +843,9 @@
       <c r="G2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="H2" s="7"/>
+      <c r="H2" s="7" t="s">
+        <v>11</v>
+      </c>
       <c r="I2" s="7"/>
       <c r="J2" s="7"/>
       <c r="K2" s="7"/>
@@ -788,7 +881,9 @@
       <c r="G3" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="H3" s="7"/>
+      <c r="H3" s="7" t="s">
+        <v>11</v>
+      </c>
       <c r="I3" s="7"/>
       <c r="J3" s="7"/>
       <c r="K3" s="7"/>
@@ -824,7 +919,9 @@
       <c r="G4" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="H4" s="7"/>
+      <c r="H4" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="I4" s="7"/>
       <c r="J4" s="7"/>
       <c r="K4" s="7"/>
@@ -860,7 +957,9 @@
       <c r="G5" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="H5" s="7"/>
+      <c r="H5" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="I5" s="7"/>
       <c r="J5" s="7"/>
       <c r="K5" s="7"/>
@@ -896,7 +995,9 @@
       <c r="G6" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="H6" s="7"/>
+      <c r="H6" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="I6" s="7"/>
       <c r="J6" s="7"/>
       <c r="K6" s="7"/>
@@ -932,7 +1033,9 @@
       <c r="G7" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="H7" s="7"/>
+      <c r="H7" s="7" t="s">
+        <v>11</v>
+      </c>
       <c r="I7" s="7"/>
       <c r="J7" s="7"/>
       <c r="K7" s="7"/>
@@ -968,7 +1071,9 @@
       <c r="G8" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="H8" s="7"/>
+      <c r="H8" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="I8" s="7"/>
       <c r="J8" s="7"/>
       <c r="K8" s="7"/>
@@ -1004,7 +1109,9 @@
       <c r="G9" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="H9" s="7"/>
+      <c r="H9" s="7" t="s">
+        <v>13</v>
+      </c>
       <c r="I9" s="7"/>
       <c r="J9" s="7"/>
       <c r="K9" s="7"/>

</xml_diff>

<commit_message>
Attendance 05 Jan 2024 & 06 Jan 2024
Attendance 05 Jan 2024 & 06 Jan 2024
</commit_message>
<xml_diff>
--- a/Project batch Sheet/Project Batch Sheet.xlsx
+++ b/Project batch Sheet/Project Batch Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Angular\JavaScript\Project batch Sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CEC8294-D33B-4161-B178-1F5AD5F9BAFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51CCE8FE-86B1-4BD8-940A-4DE81ADEEDA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{F43F5E3C-0558-E346-B770-8540CD6B4863}"/>
   </bookViews>
@@ -71,6 +71,30 @@
         </r>
       </text>
     </comment>
+    <comment ref="I2" authorId="1" shapeId="0" xr:uid="{E175E53E-6223-4755-A715-828B18311BBA}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Admin:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Extra Office Work</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="D3" authorId="0" shapeId="0" xr:uid="{0A17E92C-6FF0-4A33-A645-E6D149F8902C}">
       <text>
         <r>
@@ -140,6 +164,30 @@
           </rPr>
           <t xml:space="preserve">
 Unavailable for Meet</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J3" authorId="1" shapeId="0" xr:uid="{0AB686E4-7C85-4FFF-8C93-A534DA228328}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Admin:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Pending Assignment Completion</t>
         </r>
       </text>
     </comment>
@@ -261,6 +309,30 @@
           </rPr>
           <t xml:space="preserve">
 Relocating the Home</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J8" authorId="1" shapeId="0" xr:uid="{35865D0F-7EBC-4A35-A479-F34124694EBB}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Admin:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Family gate together</t>
         </r>
       </text>
     </comment>
@@ -293,7 +365,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="14">
   <si>
     <t>Student Name</t>
   </si>
@@ -773,7 +845,7 @@
   <dimension ref="A1:T12"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="D1:G2"/>
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -808,8 +880,12 @@
       <c r="H1" s="4">
         <v>45295</v>
       </c>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
+      <c r="I1" s="4">
+        <v>45296</v>
+      </c>
+      <c r="J1" s="4">
+        <v>45297</v>
+      </c>
       <c r="K1" s="5"/>
       <c r="L1" s="5"/>
       <c r="M1" s="5"/>
@@ -846,8 +922,12 @@
       <c r="H2" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
+      <c r="I2" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="J2" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="K2" s="7"/>
       <c r="L2" s="7"/>
       <c r="M2" s="7"/>
@@ -884,8 +964,12 @@
       <c r="H3" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="I3" s="7"/>
-      <c r="J3" s="7"/>
+      <c r="I3" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="J3" s="7" t="s">
+        <v>11</v>
+      </c>
       <c r="K3" s="7"/>
       <c r="L3" s="7"/>
       <c r="M3" s="7"/>
@@ -922,8 +1006,12 @@
       <c r="H4" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="I4" s="7"/>
-      <c r="J4" s="7"/>
+      <c r="I4" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="J4" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="K4" s="7"/>
       <c r="L4" s="7"/>
       <c r="M4" s="7"/>
@@ -960,8 +1048,12 @@
       <c r="H5" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="I5" s="7"/>
-      <c r="J5" s="7"/>
+      <c r="I5" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="J5" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="K5" s="7"/>
       <c r="L5" s="7"/>
       <c r="M5" s="7"/>
@@ -998,8 +1090,12 @@
       <c r="H6" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="I6" s="7"/>
-      <c r="J6" s="7"/>
+      <c r="I6" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="J6" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="K6" s="7"/>
       <c r="L6" s="7"/>
       <c r="M6" s="7"/>
@@ -1036,8 +1132,12 @@
       <c r="H7" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="I7" s="7"/>
-      <c r="J7" s="7"/>
+      <c r="I7" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="J7" s="7" t="s">
+        <v>13</v>
+      </c>
       <c r="K7" s="7"/>
       <c r="L7" s="7"/>
       <c r="M7" s="7"/>
@@ -1074,8 +1174,12 @@
       <c r="H8" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="I8" s="7"/>
-      <c r="J8" s="7"/>
+      <c r="I8" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="J8" s="7" t="s">
+        <v>11</v>
+      </c>
       <c r="K8" s="7"/>
       <c r="L8" s="7"/>
       <c r="M8" s="7"/>
@@ -1112,8 +1216,12 @@
       <c r="H9" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="I9" s="7"/>
-      <c r="J9" s="7"/>
+      <c r="I9" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="J9" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="K9" s="7"/>
       <c r="L9" s="7"/>
       <c r="M9" s="7"/>

</xml_diff>

<commit_message>
Attendance of 08 Jan 2024
Attendance of 08 Jan 2024
</commit_message>
<xml_diff>
--- a/Project batch Sheet/Project Batch Sheet.xlsx
+++ b/Project batch Sheet/Project Batch Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Angular\JavaScript\Project batch Sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51CCE8FE-86B1-4BD8-940A-4DE81ADEEDA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D620278D-7952-4DE7-AE2E-75A93F12BC4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{F43F5E3C-0558-E346-B770-8540CD6B4863}"/>
   </bookViews>
@@ -365,7 +365,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="14">
   <si>
     <t>Student Name</t>
   </si>
@@ -845,7 +845,7 @@
   <dimension ref="A1:T12"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -886,7 +886,9 @@
       <c r="J1" s="4">
         <v>45297</v>
       </c>
-      <c r="K1" s="5"/>
+      <c r="K1" s="4">
+        <v>45299</v>
+      </c>
       <c r="L1" s="5"/>
       <c r="M1" s="5"/>
       <c r="N1" s="5"/>
@@ -928,7 +930,9 @@
       <c r="J2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="K2" s="7"/>
+      <c r="K2" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="L2" s="7"/>
       <c r="M2" s="7"/>
       <c r="N2" s="7"/>
@@ -970,7 +974,9 @@
       <c r="J3" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="K3" s="7"/>
+      <c r="K3" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="L3" s="7"/>
       <c r="M3" s="7"/>
       <c r="N3" s="7"/>
@@ -1012,7 +1018,9 @@
       <c r="J4" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="K4" s="7"/>
+      <c r="K4" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="L4" s="7"/>
       <c r="M4" s="7"/>
       <c r="N4" s="7"/>
@@ -1054,7 +1062,9 @@
       <c r="J5" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="K5" s="7"/>
+      <c r="K5" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="L5" s="7"/>
       <c r="M5" s="7"/>
       <c r="N5" s="7"/>
@@ -1096,7 +1106,9 @@
       <c r="J6" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="K6" s="7"/>
+      <c r="K6" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="L6" s="7"/>
       <c r="M6" s="7"/>
       <c r="N6" s="7"/>
@@ -1138,7 +1150,9 @@
       <c r="J7" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="K7" s="7"/>
+      <c r="K7" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="L7" s="7"/>
       <c r="M7" s="7"/>
       <c r="N7" s="7"/>
@@ -1180,7 +1194,9 @@
       <c r="J8" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="K8" s="7"/>
+      <c r="K8" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="L8" s="7"/>
       <c r="M8" s="7"/>
       <c r="N8" s="7"/>
@@ -1222,7 +1238,9 @@
       <c r="J9" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="K9" s="7"/>
+      <c r="K9" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="L9" s="7"/>
       <c r="M9" s="7"/>
       <c r="N9" s="7"/>

</xml_diff>

<commit_message>
Google Meet Attendance 09 , 10 & 11 Jan 2024
Google Meet Attendance 09 , 10 & 11 Jan 2024
</commit_message>
<xml_diff>
--- a/Project batch Sheet/Project Batch Sheet.xlsx
+++ b/Project batch Sheet/Project Batch Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Angular\JavaScript\Project batch Sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D620278D-7952-4DE7-AE2E-75A93F12BC4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{453B515F-E5A9-45AE-96DE-D0ADD26A7626}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{F43F5E3C-0558-E346-B770-8540CD6B4863}"/>
   </bookViews>
@@ -95,6 +95,30 @@
         </r>
       </text>
     </comment>
+    <comment ref="L2" authorId="1" shapeId="0" xr:uid="{743FC7FD-6BFF-46F1-9425-37C90B4144F2}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Admin:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Health Issue</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="D3" authorId="0" shapeId="0" xr:uid="{0A17E92C-6FF0-4A33-A645-E6D149F8902C}">
       <text>
         <r>
@@ -191,6 +215,30 @@
         </r>
       </text>
     </comment>
+    <comment ref="L3" authorId="1" shapeId="0" xr:uid="{39DDA81C-12E6-43FC-995F-24B95F994BC2}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Admin:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Office Work</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="E5" authorId="0" shapeId="0" xr:uid="{E1A6D40D-C230-4FE8-BAE1-D6B369291E94}">
       <text>
         <r>
@@ -236,6 +284,30 @@
           </rPr>
           <t xml:space="preserve">
 Health Issue</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M6" authorId="1" shapeId="0" xr:uid="{A2A42A80-6967-46AD-A75E-3ED5FA8A424D}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Admin:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Family Emergency</t>
         </r>
       </text>
     </comment>
@@ -336,6 +408,31 @@
         </r>
       </text>
     </comment>
+    <comment ref="L8" authorId="1" shapeId="0" xr:uid="{D50D437E-2512-4C07-8167-64B02121B97A}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Admin:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Family Function
+</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="H9" authorId="1" shapeId="0" xr:uid="{878DF12F-2629-4626-9ED2-8FCBC10AFEBF}">
       <text>
         <r>
@@ -357,6 +454,31 @@
           </rPr>
           <t xml:space="preserve">
 Travelling</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="L9" authorId="1" shapeId="0" xr:uid="{8181D3D5-2C22-4FDD-8D5C-21780DAFFE74}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Admin:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Network Issue
+</t>
         </r>
       </text>
     </comment>
@@ -365,7 +487,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="14">
   <si>
     <t>Student Name</t>
   </si>
@@ -845,7 +967,7 @@
   <dimension ref="A1:T12"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+      <selection activeCell="K16" activeCellId="1" sqref="L11 K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -889,9 +1011,15 @@
       <c r="K1" s="4">
         <v>45299</v>
       </c>
-      <c r="L1" s="5"/>
-      <c r="M1" s="5"/>
-      <c r="N1" s="5"/>
+      <c r="L1" s="4">
+        <v>45300</v>
+      </c>
+      <c r="M1" s="4">
+        <v>45301</v>
+      </c>
+      <c r="N1" s="4">
+        <v>45302</v>
+      </c>
       <c r="O1" s="5"/>
       <c r="P1" s="5"/>
       <c r="Q1" s="5"/>
@@ -933,9 +1061,15 @@
       <c r="K2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="L2" s="7"/>
-      <c r="M2" s="7"/>
-      <c r="N2" s="7"/>
+      <c r="L2" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="M2" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="N2" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="O2" s="7"/>
       <c r="P2" s="7"/>
       <c r="Q2" s="7"/>
@@ -977,9 +1111,15 @@
       <c r="K3" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="L3" s="7"/>
-      <c r="M3" s="7"/>
-      <c r="N3" s="7"/>
+      <c r="L3" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="M3" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="N3" s="7" t="s">
+        <v>13</v>
+      </c>
       <c r="O3" s="7"/>
       <c r="P3" s="7"/>
       <c r="Q3" s="7"/>
@@ -1021,9 +1161,15 @@
       <c r="K4" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="L4" s="7"/>
-      <c r="M4" s="7"/>
-      <c r="N4" s="7"/>
+      <c r="L4" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="M4" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="N4" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="O4" s="7"/>
       <c r="P4" s="7"/>
       <c r="Q4" s="7"/>
@@ -1065,9 +1211,15 @@
       <c r="K5" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="L5" s="7"/>
-      <c r="M5" s="7"/>
-      <c r="N5" s="7"/>
+      <c r="L5" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="M5" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="N5" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="O5" s="7"/>
       <c r="P5" s="7"/>
       <c r="Q5" s="7"/>
@@ -1109,9 +1261,15 @@
       <c r="K6" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="L6" s="7"/>
-      <c r="M6" s="7"/>
-      <c r="N6" s="7"/>
+      <c r="L6" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="M6" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="N6" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="O6" s="7"/>
       <c r="P6" s="7"/>
       <c r="Q6" s="7"/>
@@ -1153,9 +1311,15 @@
       <c r="K7" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="L7" s="7"/>
-      <c r="M7" s="7"/>
-      <c r="N7" s="7"/>
+      <c r="L7" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="M7" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="N7" s="7" t="s">
+        <v>13</v>
+      </c>
       <c r="O7" s="7"/>
       <c r="P7" s="7"/>
       <c r="Q7" s="7"/>
@@ -1197,9 +1361,15 @@
       <c r="K8" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="L8" s="7"/>
-      <c r="M8" s="7"/>
-      <c r="N8" s="7"/>
+      <c r="L8" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="M8" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="N8" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="O8" s="7"/>
       <c r="P8" s="7"/>
       <c r="Q8" s="7"/>
@@ -1241,9 +1411,15 @@
       <c r="K9" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="L9" s="7"/>
-      <c r="M9" s="7"/>
-      <c r="N9" s="7"/>
+      <c r="L9" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="M9" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="N9" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="O9" s="7"/>
       <c r="P9" s="7"/>
       <c r="Q9" s="7"/>

</xml_diff>

<commit_message>
attendance on 12 Jan 2024
attendance on 12 Jan 2024
</commit_message>
<xml_diff>
--- a/Project batch Sheet/Project Batch Sheet.xlsx
+++ b/Project batch Sheet/Project Batch Sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Angular\JavaScript\Project batch Sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{453B515F-E5A9-45AE-96DE-D0ADD26A7626}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60185B4E-C128-4CA0-8D56-B33E9879CD1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{F43F5E3C-0558-E346-B770-8540CD6B4863}"/>
+    <workbookView xWindow="1080" yWindow="1080" windowWidth="15375" windowHeight="7875" xr2:uid="{F43F5E3C-0558-E346-B770-8540CD6B4863}"/>
   </bookViews>
   <sheets>
     <sheet name="Dec-2023" sheetId="1" r:id="rId1"/>
@@ -384,6 +384,30 @@
         </r>
       </text>
     </comment>
+    <comment ref="O7" authorId="1" shapeId="0" xr:uid="{D5F51D3E-DE13-4EE9-84C4-700826210C5B}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Admin:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve"> travelling</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="J8" authorId="1" shapeId="0" xr:uid="{35865D0F-7EBC-4A35-A479-F34124694EBB}">
       <text>
         <r>
@@ -487,7 +511,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="20">
   <si>
     <t>Student Name</t>
   </si>
@@ -529,6 +553,24 @@
   </si>
   <si>
     <t>Absent</t>
+  </si>
+  <si>
+    <t>Discussion Points:</t>
+  </si>
+  <si>
+    <t>10 mints : Hr Introduction</t>
+  </si>
+  <si>
+    <t>15 Mints : PPT Presention on Particular Topic</t>
+  </si>
+  <si>
+    <t>15 mints: Question &amp; Answer Session</t>
+  </si>
+  <si>
+    <t>15 Mints : Assignment Quaries &amp; lecture Discussion</t>
+  </si>
+  <si>
+    <t>5 mint: Tomorrow Meet Discussion Points</t>
   </si>
 </sst>
 </file>
@@ -585,7 +627,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -601,6 +643,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -632,7 +680,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -648,6 +696,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -964,16 +1015,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF336CF2-9F7E-9D47-A242-C3CB362C49F8}">
-  <dimension ref="A1:T12"/>
+  <dimension ref="A1:T19"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="K16" activeCellId="1" sqref="L11 K16"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6.125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="44.125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1020,7 +1071,9 @@
       <c r="N1" s="4">
         <v>45302</v>
       </c>
-      <c r="O1" s="5"/>
+      <c r="O1" s="4">
+        <v>45303</v>
+      </c>
       <c r="P1" s="5"/>
       <c r="Q1" s="5"/>
       <c r="R1" s="5"/>
@@ -1070,7 +1123,9 @@
       <c r="N2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="O2" s="7"/>
+      <c r="O2" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="P2" s="7"/>
       <c r="Q2" s="7"/>
       <c r="R2" s="7"/>
@@ -1120,7 +1175,9 @@
       <c r="N3" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="O3" s="7"/>
+      <c r="O3" s="7" t="s">
+        <v>13</v>
+      </c>
       <c r="P3" s="7"/>
       <c r="Q3" s="7"/>
       <c r="R3" s="7"/>
@@ -1170,7 +1227,9 @@
       <c r="N4" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="O4" s="7"/>
+      <c r="O4" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="P4" s="7"/>
       <c r="Q4" s="7"/>
       <c r="R4" s="7"/>
@@ -1220,7 +1279,9 @@
       <c r="N5" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="O5" s="7"/>
+      <c r="O5" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="P5" s="7"/>
       <c r="Q5" s="7"/>
       <c r="R5" s="7"/>
@@ -1270,7 +1331,9 @@
       <c r="N6" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="O6" s="7"/>
+      <c r="O6" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="P6" s="7"/>
       <c r="Q6" s="7"/>
       <c r="R6" s="7"/>
@@ -1320,7 +1383,9 @@
       <c r="N7" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="O7" s="7"/>
+      <c r="O7" s="7" t="s">
+        <v>11</v>
+      </c>
       <c r="P7" s="7"/>
       <c r="Q7" s="7"/>
       <c r="R7" s="7"/>
@@ -1370,7 +1435,9 @@
       <c r="N8" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="O8" s="7"/>
+      <c r="O8" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="P8" s="7"/>
       <c r="Q8" s="7"/>
       <c r="R8" s="7"/>
@@ -1420,7 +1487,9 @@
       <c r="N9" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="O9" s="7"/>
+      <c r="O9" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="P9" s="7"/>
       <c r="Q9" s="7"/>
       <c r="R9" s="7"/>
@@ -1432,9 +1501,39 @@
         <v>3</v>
       </c>
     </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B14" s="9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B15" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B16" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B17" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B18" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B19" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:N9" xr:uid="{F036FACA-372A-8349-BD3D-950830E988A4}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:T9" xr:uid="{F036FACA-372A-8349-BD3D-950830E988A4}">
       <formula1>"Present, Absent,Reason"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
attendance 13 Jan  2024 to 22 Jan 2024
attendance 13 Jan  2024 to 22 Jan 2024
</commit_message>
<xml_diff>
--- a/Project batch Sheet/Project Batch Sheet.xlsx
+++ b/Project batch Sheet/Project Batch Sheet.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20406"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Angular\JavaScript\Project batch Sheet\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kisho\OneDrive\Desktop\Data\Angular\JavaScript\Project batch Sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60185B4E-C128-4CA0-8D56-B33E9879CD1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D462894-5EFD-43A1-91B1-889FF5AF4B5E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1080" yWindow="1080" windowWidth="15375" windowHeight="7875" xr2:uid="{F43F5E3C-0558-E346-B770-8540CD6B4863}"/>
   </bookViews>
@@ -29,6 +29,7 @@
   <authors>
     <author>Hp</author>
     <author>Admin</author>
+    <author>K K</author>
   </authors>
   <commentList>
     <comment ref="E2" authorId="0" shapeId="0" xr:uid="{DB85F54B-2016-4DCB-8ED7-68D1B5D97712}">
@@ -119,6 +120,30 @@
         </r>
       </text>
     </comment>
+    <comment ref="S2" authorId="2" shapeId="0" xr:uid="{2C3E7B29-77DB-4F48-B4CD-3AF6EEAC9CFE}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>K K:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Assignment Completion</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="D3" authorId="0" shapeId="0" xr:uid="{0A17E92C-6FF0-4A33-A645-E6D149F8902C}">
       <text>
         <r>
@@ -239,6 +264,102 @@
         </r>
       </text>
     </comment>
+    <comment ref="N3" authorId="2" shapeId="0" xr:uid="{28002F0A-5CED-46C9-9450-129528379ABA}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>K K:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Assignment Completion</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="O3" authorId="2" shapeId="0" xr:uid="{09C7F255-47E2-4960-9615-10FCA7BC569A}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>K K:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Assignment Completion</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="P3" authorId="2" shapeId="0" xr:uid="{C563A402-EE5F-4F0A-A852-459AF3402BAE}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>K K:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Assignment Completion</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="R3" authorId="2" shapeId="0" xr:uid="{CA1D262C-F198-42E9-B2F0-6B3C37289A21}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>K K:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Network Issue</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="E5" authorId="0" shapeId="0" xr:uid="{E1A6D40D-C230-4FE8-BAE1-D6B369291E94}">
       <text>
         <r>
@@ -308,6 +429,30 @@
           </rPr>
           <t xml:space="preserve">
 Family Emergency</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="W6" authorId="1" shapeId="0" xr:uid="{8581658A-E140-4E0F-B83F-9D5CA9E7AA7D}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Admin:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve"> travelling</t>
         </r>
       </text>
     </comment>
@@ -408,6 +553,54 @@
         </r>
       </text>
     </comment>
+    <comment ref="P7" authorId="2" shapeId="0" xr:uid="{2A8C016F-85BE-4CB2-9C98-FAEBD85DD429}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>K K:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Network Issue</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="S7" authorId="2" shapeId="0" xr:uid="{E0F97DED-17C2-4049-BCCB-5BD1809E5294}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>K K:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Office Issue</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="J8" authorId="1" shapeId="0" xr:uid="{35865D0F-7EBC-4A35-A479-F34124694EBB}">
       <text>
         <r>
@@ -457,6 +650,30 @@
         </r>
       </text>
     </comment>
+    <comment ref="W8" authorId="2" shapeId="0" xr:uid="{B636F89C-B4EC-455A-BFDE-D6BC08F8C6CB}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>K K:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Health issue</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="H9" authorId="1" shapeId="0" xr:uid="{878DF12F-2629-4626-9ED2-8FCBC10AFEBF}">
       <text>
         <r>
@@ -503,6 +720,126 @@
           <t xml:space="preserve">
 Network Issue
 </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="S9" authorId="2" shapeId="0" xr:uid="{C59A3634-0A00-4967-9099-C342AE6BD492}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>K K:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Eye Operation</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="T9" authorId="2" shapeId="0" xr:uid="{C61FF010-F2CE-49EC-B70B-0A6A10679C19}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>K K:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Eye Operation</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="U9" authorId="2" shapeId="0" xr:uid="{E3EC8ABF-0AA7-4B02-BAE7-8FFF94624E23}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>K K:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Eye Operation</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="V9" authorId="2" shapeId="0" xr:uid="{D547BBA1-785F-40DB-8337-29226ADF3B74}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>K K:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Eye Operation</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="W9" authorId="2" shapeId="0" xr:uid="{615A4314-702E-4D6A-9DEA-0648E5B35A7F}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>K K:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Eye Operation</t>
         </r>
       </text>
     </comment>
@@ -511,7 +848,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="20">
   <si>
     <t>Student Name</t>
   </si>
@@ -577,7 +914,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -625,6 +962,19 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="5">
@@ -680,7 +1030,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -690,7 +1040,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="15" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1015,10 +1364,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF336CF2-9F7E-9D47-A242-C3CB362C49F8}">
-  <dimension ref="A1:T19"/>
+  <dimension ref="A1:Z19"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="S19" sqref="S19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1028,7 +1377,7 @@
     <col min="4" max="4" width="11.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:26" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -1074,444 +1423,639 @@
       <c r="O1" s="4">
         <v>45303</v>
       </c>
-      <c r="P1" s="5"/>
-      <c r="Q1" s="5"/>
-      <c r="R1" s="5"/>
-      <c r="S1" s="5"/>
-      <c r="T1" s="5"/>
+      <c r="P1" s="4">
+        <v>45304</v>
+      </c>
+      <c r="Q1" s="4">
+        <v>45306</v>
+      </c>
+      <c r="R1" s="4">
+        <v>45307</v>
+      </c>
+      <c r="S1" s="4">
+        <v>45308</v>
+      </c>
+      <c r="T1" s="4">
+        <v>45309</v>
+      </c>
+      <c r="U1" s="4">
+        <v>45310</v>
+      </c>
+      <c r="V1" s="4">
+        <v>45311</v>
+      </c>
+      <c r="W1" s="4">
+        <v>45313</v>
+      </c>
     </row>
-    <row r="2" spans="1:20" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A2" s="6">
+    <row r="2" spans="1:26" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A2" s="5">
         <v>1</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="H2" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="I2" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="J2" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="K2" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="L2" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="M2" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="N2" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="O2" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="P2" s="7"/>
-      <c r="Q2" s="7"/>
-      <c r="R2" s="7"/>
-      <c r="S2" s="7"/>
-      <c r="T2" s="7"/>
+      <c r="C2" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="K2" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="L2" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="M2" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="N2" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="O2" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="P2" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q2" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="R2" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="S2" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="T2" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="U2" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="V2" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="W2" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="X2" s="6"/>
+      <c r="Y2" s="6"/>
+      <c r="Z2" s="6"/>
     </row>
-    <row r="3" spans="1:20" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A3" s="6">
-        <v>2</v>
-      </c>
-      <c r="B3" s="6" t="s">
+    <row r="3" spans="1:26" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A3" s="5">
+        <v>2</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="G3" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="H3" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="I3" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="J3" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="K3" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="L3" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="M3" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="N3" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="O3" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="P3" s="7"/>
-      <c r="Q3" s="7"/>
-      <c r="R3" s="7"/>
-      <c r="S3" s="7"/>
-      <c r="T3" s="7"/>
+      <c r="C3" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="J3" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="K3" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="L3" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="M3" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="N3" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="O3" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="P3" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q3" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="R3" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="S3" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="T3" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="U3" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="V3" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="W3" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="X3" s="6"/>
+      <c r="Y3" s="6"/>
+      <c r="Z3" s="6"/>
     </row>
-    <row r="4" spans="1:20" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A4" s="6">
+    <row r="4" spans="1:26" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A4" s="5">
         <v>3</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="F4" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="G4" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="H4" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="I4" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="J4" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="K4" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="L4" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="M4" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="N4" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="O4" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="P4" s="7"/>
-      <c r="Q4" s="7"/>
-      <c r="R4" s="7"/>
-      <c r="S4" s="7"/>
-      <c r="T4" s="7"/>
+      <c r="C4" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="I4" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="J4" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="K4" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="L4" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="M4" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="N4" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="O4" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="P4" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q4" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="R4" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="S4" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="T4" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="U4" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="V4" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="W4" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="X4" s="6"/>
+      <c r="Y4" s="6"/>
+      <c r="Z4" s="6"/>
     </row>
-    <row r="5" spans="1:20" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A5" s="6">
+    <row r="5" spans="1:26" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A5" s="5">
         <v>4</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="F5" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="G5" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="H5" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="I5" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="J5" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="K5" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="L5" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="M5" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="N5" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="O5" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="P5" s="7"/>
-      <c r="Q5" s="7"/>
-      <c r="R5" s="7"/>
-      <c r="S5" s="7"/>
-      <c r="T5" s="7"/>
+      <c r="C5" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="I5" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="J5" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="K5" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="L5" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="M5" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="N5" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="O5" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="P5" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q5" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="R5" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="S5" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="T5" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="U5" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="V5" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="W5" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="X5" s="6"/>
+      <c r="Y5" s="6"/>
+      <c r="Z5" s="6"/>
     </row>
-    <row r="6" spans="1:20" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A6" s="6">
+    <row r="6" spans="1:26" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A6" s="5">
         <v>5</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="F6" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="G6" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="H6" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="I6" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="J6" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="K6" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="L6" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="M6" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="N6" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="O6" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="P6" s="7"/>
-      <c r="Q6" s="7"/>
-      <c r="R6" s="7"/>
-      <c r="S6" s="7"/>
-      <c r="T6" s="7"/>
+      <c r="C6" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="I6" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="J6" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="K6" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="L6" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="M6" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="N6" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="O6" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="P6" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q6" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="R6" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="S6" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="T6" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="U6" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="V6" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="W6" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="X6" s="6"/>
+      <c r="Y6" s="6"/>
+      <c r="Z6" s="6"/>
     </row>
-    <row r="7" spans="1:20" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A7" s="6">
+    <row r="7" spans="1:26" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A7" s="5">
         <v>6</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="E7" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="F7" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="G7" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="H7" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="I7" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="J7" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="K7" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="L7" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="M7" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="N7" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="O7" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="P7" s="7"/>
-      <c r="Q7" s="7"/>
-      <c r="R7" s="7"/>
-      <c r="S7" s="7"/>
-      <c r="T7" s="7"/>
+      <c r="C7" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="I7" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="J7" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="K7" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="L7" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="M7" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="N7" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="O7" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="P7" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q7" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="R7" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="S7" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="T7" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="U7" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="V7" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="W7" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="X7" s="6"/>
+      <c r="Y7" s="6"/>
+      <c r="Z7" s="6"/>
     </row>
-    <row r="8" spans="1:20" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A8" s="6">
+    <row r="8" spans="1:26" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A8" s="5">
         <v>7</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="E8" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="F8" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="G8" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="H8" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="I8" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="J8" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="K8" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="L8" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="M8" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="N8" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="O8" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="P8" s="7"/>
-      <c r="Q8" s="7"/>
-      <c r="R8" s="7"/>
-      <c r="S8" s="7"/>
-      <c r="T8" s="7"/>
+      <c r="C8" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="I8" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="J8" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="K8" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="L8" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="M8" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="N8" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="O8" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="P8" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q8" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="R8" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="S8" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="T8" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="U8" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="V8" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="W8" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="X8" s="6"/>
+      <c r="Y8" s="6"/>
+      <c r="Z8" s="6"/>
     </row>
-    <row r="9" spans="1:20" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A9" s="6">
+    <row r="9" spans="1:26" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A9" s="5">
         <v>8</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="F9" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="G9" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="H9" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="I9" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="J9" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="K9" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="L9" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="M9" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="N9" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="O9" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="P9" s="7"/>
-      <c r="Q9" s="7"/>
-      <c r="R9" s="7"/>
-      <c r="S9" s="7"/>
-      <c r="T9" s="7"/>
+      <c r="C9" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="I9" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="J9" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="K9" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="L9" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="M9" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="N9" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="O9" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="P9" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q9" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="R9" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="S9" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="T9" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="U9" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="V9" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="W9" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="X9" s="6"/>
+      <c r="Y9" s="6"/>
+      <c r="Z9" s="6"/>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B12" s="8" t="s">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="B12" s="7" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B14" s="9" t="s">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="B14" s="8" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
         <v>16</v>
       </c>
@@ -1533,7 +2077,7 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:T9" xr:uid="{F036FACA-372A-8349-BD3D-950830E988A4}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:Z9" xr:uid="{F036FACA-372A-8349-BD3D-950830E988A4}">
       <formula1>"Present, Absent,Reason"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
23 Jan & 24 Jan 2024 Attendance
23 Jan & 24 Jan 2024 Attendance
</commit_message>
<xml_diff>
--- a/Project batch Sheet/Project Batch Sheet.xlsx
+++ b/Project batch Sheet/Project Batch Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kisho\OneDrive\Desktop\Data\Angular\JavaScript\Project batch Sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D462894-5EFD-43A1-91B1-889FF5AF4B5E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECE39B02-D224-49A8-B556-F18A06F1C68B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1080" yWindow="1080" windowWidth="15375" windowHeight="7875" xr2:uid="{F43F5E3C-0558-E346-B770-8540CD6B4863}"/>
   </bookViews>
@@ -456,6 +456,54 @@
         </r>
       </text>
     </comment>
+    <comment ref="X6" authorId="2" shapeId="0" xr:uid="{3920E565-A2B0-43D8-B260-E96E0C1B8FC6}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>K K:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Not In Town</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="Y6" authorId="2" shapeId="0" xr:uid="{49FCD233-A720-4861-9731-E379355AE280}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>K K:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Not In Town</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="D7" authorId="0" shapeId="0" xr:uid="{537A38CA-D15F-4AB4-A182-B03C454B3293}">
       <text>
         <r>
@@ -820,6 +868,54 @@
       </text>
     </comment>
     <comment ref="W9" authorId="2" shapeId="0" xr:uid="{615A4314-702E-4D6A-9DEA-0648E5B35A7F}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>K K:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Eye Operation</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="X9" authorId="2" shapeId="0" xr:uid="{77BE6059-8846-429E-A76D-427F49351ECD}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>K K:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Eye Operation</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="Y9" authorId="2" shapeId="0" xr:uid="{5BA8BB17-A007-4EAD-BEC0-F1629DF58178}">
       <text>
         <r>
           <rPr>
@@ -848,7 +944,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="20">
   <si>
     <t>Student Name</t>
   </si>
@@ -1367,7 +1463,7 @@
   <dimension ref="A1:Z19"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="S19" sqref="S19"/>
+      <selection activeCell="U16" sqref="U16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1447,6 +1543,12 @@
       <c r="W1" s="4">
         <v>45313</v>
       </c>
+      <c r="X1" s="4">
+        <v>45314</v>
+      </c>
+      <c r="Y1" s="4">
+        <v>45315</v>
+      </c>
     </row>
     <row r="2" spans="1:26" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="5">
@@ -1518,8 +1620,12 @@
       <c r="W2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="X2" s="6"/>
-      <c r="Y2" s="6"/>
+      <c r="X2" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y2" s="6" t="s">
+        <v>2</v>
+      </c>
       <c r="Z2" s="6"/>
     </row>
     <row r="3" spans="1:26" ht="18.75" x14ac:dyDescent="0.3">
@@ -1592,8 +1698,12 @@
       <c r="W3" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="X3" s="6"/>
-      <c r="Y3" s="6"/>
+      <c r="X3" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y3" s="6" t="s">
+        <v>2</v>
+      </c>
       <c r="Z3" s="6"/>
     </row>
     <row r="4" spans="1:26" ht="18.75" x14ac:dyDescent="0.3">
@@ -1666,8 +1776,12 @@
       <c r="W4" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="X4" s="6"/>
-      <c r="Y4" s="6"/>
+      <c r="X4" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y4" s="6" t="s">
+        <v>2</v>
+      </c>
       <c r="Z4" s="6"/>
     </row>
     <row r="5" spans="1:26" ht="18.75" x14ac:dyDescent="0.3">
@@ -1740,8 +1854,12 @@
       <c r="W5" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="X5" s="6"/>
-      <c r="Y5" s="6"/>
+      <c r="X5" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y5" s="6" t="s">
+        <v>2</v>
+      </c>
       <c r="Z5" s="6"/>
     </row>
     <row r="6" spans="1:26" ht="18.75" x14ac:dyDescent="0.3">
@@ -1814,8 +1932,12 @@
       <c r="W6" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="X6" s="6"/>
-      <c r="Y6" s="6"/>
+      <c r="X6" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="Y6" s="6" t="s">
+        <v>11</v>
+      </c>
       <c r="Z6" s="6"/>
     </row>
     <row r="7" spans="1:26" ht="18.75" x14ac:dyDescent="0.3">
@@ -1888,8 +2010,12 @@
       <c r="W7" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="X7" s="6"/>
-      <c r="Y7" s="6"/>
+      <c r="X7" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y7" s="6" t="s">
+        <v>13</v>
+      </c>
       <c r="Z7" s="6"/>
     </row>
     <row r="8" spans="1:26" ht="18.75" x14ac:dyDescent="0.3">
@@ -1962,8 +2088,12 @@
       <c r="W8" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="X8" s="6"/>
-      <c r="Y8" s="6"/>
+      <c r="X8" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y8" s="6" t="s">
+        <v>2</v>
+      </c>
       <c r="Z8" s="6"/>
     </row>
     <row r="9" spans="1:26" ht="18.75" x14ac:dyDescent="0.3">
@@ -2036,8 +2166,12 @@
       <c r="W9" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="X9" s="6"/>
-      <c r="Y9" s="6"/>
+      <c r="X9" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="Y9" s="6" t="s">
+        <v>11</v>
+      </c>
       <c r="Z9" s="6"/>
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
attendance of 25th Jan & 26th Jan 2024
attendance of 25th Jan & 26th Jan 2024
</commit_message>
<xml_diff>
--- a/Project batch Sheet/Project Batch Sheet.xlsx
+++ b/Project batch Sheet/Project Batch Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kisho\OneDrive\Desktop\Data\Angular\JavaScript\Project batch Sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECE39B02-D224-49A8-B556-F18A06F1C68B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F73E8F8-F8FC-488E-A8CD-C8287409C5A6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1080" yWindow="1080" windowWidth="15375" windowHeight="7875" xr2:uid="{F43F5E3C-0558-E346-B770-8540CD6B4863}"/>
   </bookViews>
@@ -144,6 +144,30 @@
         </r>
       </text>
     </comment>
+    <comment ref="Z2" authorId="2" shapeId="0" xr:uid="{6611BE39-6804-46DA-99A5-0BAB7D795D77}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>K K:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Go Outside</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="D3" authorId="0" shapeId="0" xr:uid="{0A17E92C-6FF0-4A33-A645-E6D149F8902C}">
       <text>
         <r>
@@ -916,6 +940,54 @@
       </text>
     </comment>
     <comment ref="Y9" authorId="2" shapeId="0" xr:uid="{5BA8BB17-A007-4EAD-BEC0-F1629DF58178}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>K K:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Eye Operation</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="Z9" authorId="2" shapeId="0" xr:uid="{1DCA9C82-1BAF-4FC9-A7A8-ED37D7E43642}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>K K:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Eye Operation</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AA9" authorId="2" shapeId="0" xr:uid="{2FDBA586-EB58-4409-ABB3-7069A87198CA}">
       <text>
         <r>
           <rPr>
@@ -944,7 +1016,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="20">
   <si>
     <t>Student Name</t>
   </si>
@@ -1460,10 +1532,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF336CF2-9F7E-9D47-A242-C3CB362C49F8}">
-  <dimension ref="A1:Z19"/>
+  <dimension ref="A1:AL19"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="U16" sqref="U16"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="AC5" sqref="AC5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1473,7 +1545,7 @@
     <col min="4" max="4" width="11.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:38" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -1549,8 +1621,14 @@
       <c r="Y1" s="4">
         <v>45315</v>
       </c>
+      <c r="Z1" s="4">
+        <v>45316</v>
+      </c>
+      <c r="AA1" s="4">
+        <v>45317</v>
+      </c>
     </row>
-    <row r="2" spans="1:26" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:38" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -1626,9 +1704,25 @@
       <c r="Y2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="Z2" s="6"/>
+      <c r="Z2" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="AA2" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="AB2" s="6"/>
+      <c r="AC2" s="6"/>
+      <c r="AD2" s="6"/>
+      <c r="AE2" s="6"/>
+      <c r="AF2" s="6"/>
+      <c r="AG2" s="6"/>
+      <c r="AH2" s="6"/>
+      <c r="AI2" s="6"/>
+      <c r="AJ2" s="6"/>
+      <c r="AK2" s="6"/>
+      <c r="AL2" s="6"/>
     </row>
-    <row r="3" spans="1:26" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:38" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="5">
         <v>2</v>
       </c>
@@ -1704,9 +1798,25 @@
       <c r="Y3" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="Z3" s="6"/>
+      <c r="Z3" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="AA3" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="AB3" s="6"/>
+      <c r="AC3" s="6"/>
+      <c r="AD3" s="6"/>
+      <c r="AE3" s="6"/>
+      <c r="AF3" s="6"/>
+      <c r="AG3" s="6"/>
+      <c r="AH3" s="6"/>
+      <c r="AI3" s="6"/>
+      <c r="AJ3" s="6"/>
+      <c r="AK3" s="6"/>
+      <c r="AL3" s="6"/>
     </row>
-    <row r="4" spans="1:26" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:38" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A4" s="5">
         <v>3</v>
       </c>
@@ -1782,9 +1892,25 @@
       <c r="Y4" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="Z4" s="6"/>
+      <c r="Z4" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="AA4" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="AB4" s="6"/>
+      <c r="AC4" s="6"/>
+      <c r="AD4" s="6"/>
+      <c r="AE4" s="6"/>
+      <c r="AF4" s="6"/>
+      <c r="AG4" s="6"/>
+      <c r="AH4" s="6"/>
+      <c r="AI4" s="6"/>
+      <c r="AJ4" s="6"/>
+      <c r="AK4" s="6"/>
+      <c r="AL4" s="6"/>
     </row>
-    <row r="5" spans="1:26" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:38" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A5" s="5">
         <v>4</v>
       </c>
@@ -1860,9 +1986,25 @@
       <c r="Y5" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="Z5" s="6"/>
+      <c r="Z5" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="AA5" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB5" s="6"/>
+      <c r="AC5" s="6"/>
+      <c r="AD5" s="6"/>
+      <c r="AE5" s="6"/>
+      <c r="AF5" s="6"/>
+      <c r="AG5" s="6"/>
+      <c r="AH5" s="6"/>
+      <c r="AI5" s="6"/>
+      <c r="AJ5" s="6"/>
+      <c r="AK5" s="6"/>
+      <c r="AL5" s="6"/>
     </row>
-    <row r="6" spans="1:26" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:38" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A6" s="5">
         <v>5</v>
       </c>
@@ -1938,9 +2080,25 @@
       <c r="Y6" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="Z6" s="6"/>
+      <c r="Z6" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="AA6" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="AB6" s="6"/>
+      <c r="AC6" s="6"/>
+      <c r="AD6" s="6"/>
+      <c r="AE6" s="6"/>
+      <c r="AF6" s="6"/>
+      <c r="AG6" s="6"/>
+      <c r="AH6" s="6"/>
+      <c r="AI6" s="6"/>
+      <c r="AJ6" s="6"/>
+      <c r="AK6" s="6"/>
+      <c r="AL6" s="6"/>
     </row>
-    <row r="7" spans="1:26" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:38" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A7" s="5">
         <v>6</v>
       </c>
@@ -2016,9 +2174,25 @@
       <c r="Y7" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="Z7" s="6"/>
+      <c r="Z7" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA7" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB7" s="6"/>
+      <c r="AC7" s="6"/>
+      <c r="AD7" s="6"/>
+      <c r="AE7" s="6"/>
+      <c r="AF7" s="6"/>
+      <c r="AG7" s="6"/>
+      <c r="AH7" s="6"/>
+      <c r="AI7" s="6"/>
+      <c r="AJ7" s="6"/>
+      <c r="AK7" s="6"/>
+      <c r="AL7" s="6"/>
     </row>
-    <row r="8" spans="1:26" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:38" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A8" s="5">
         <v>7</v>
       </c>
@@ -2094,9 +2268,25 @@
       <c r="Y8" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="Z8" s="6"/>
+      <c r="Z8" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="AA8" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="AB8" s="6"/>
+      <c r="AC8" s="6"/>
+      <c r="AD8" s="6"/>
+      <c r="AE8" s="6"/>
+      <c r="AF8" s="6"/>
+      <c r="AG8" s="6"/>
+      <c r="AH8" s="6"/>
+      <c r="AI8" s="6"/>
+      <c r="AJ8" s="6"/>
+      <c r="AK8" s="6"/>
+      <c r="AL8" s="6"/>
     </row>
-    <row r="9" spans="1:26" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:38" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A9" s="5">
         <v>8</v>
       </c>
@@ -2172,24 +2362,40 @@
       <c r="Y9" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="Z9" s="6"/>
+      <c r="Z9" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="AA9" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="AB9" s="6"/>
+      <c r="AC9" s="6"/>
+      <c r="AD9" s="6"/>
+      <c r="AE9" s="6"/>
+      <c r="AF9" s="6"/>
+      <c r="AG9" s="6"/>
+      <c r="AH9" s="6"/>
+      <c r="AI9" s="6"/>
+      <c r="AJ9" s="6"/>
+      <c r="AK9" s="6"/>
+      <c r="AL9" s="6"/>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:38" x14ac:dyDescent="0.25">
       <c r="B12" s="7" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:38" x14ac:dyDescent="0.25">
       <c r="B14" s="8" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:38" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:38" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
         <v>16</v>
       </c>
@@ -2211,7 +2417,7 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:Z9" xr:uid="{F036FACA-372A-8349-BD3D-950830E988A4}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:AL9" xr:uid="{F036FACA-372A-8349-BD3D-950830E988A4}">
       <formula1>"Present, Absent,Reason"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Attendance from 27 Jan to 8 Feb 2024
Attendance from 27 Jan to 8 Feb 2024
</commit_message>
<xml_diff>
--- a/Project batch Sheet/Project Batch Sheet.xlsx
+++ b/Project batch Sheet/Project Batch Sheet.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kisho\OneDrive\Desktop\Data\Angular\JavaScript\Project batch Sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F73E8F8-F8FC-488E-A8CD-C8287409C5A6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C03A875-7D4E-423F-BC9F-124878A77DDB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1080" yWindow="1080" windowWidth="15375" windowHeight="7875" xr2:uid="{F43F5E3C-0558-E346-B770-8540CD6B4863}"/>
+    <workbookView xWindow="1080" yWindow="1080" windowWidth="15375" windowHeight="7875" activeTab="1" xr2:uid="{F43F5E3C-0558-E346-B770-8540CD6B4863}"/>
   </bookViews>
   <sheets>
     <sheet name="Dec-2023" sheetId="1" r:id="rId1"/>
+    <sheet name="Feb 2024" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -168,6 +169,54 @@
         </r>
       </text>
     </comment>
+    <comment ref="AD2" authorId="2" shapeId="0" xr:uid="{C04F12EC-DB8C-489B-9163-B6AA201A1263}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>K K:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Mock Interview Prepartion</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AE2" authorId="2" shapeId="0" xr:uid="{A0415645-E4AC-4F4C-A591-8D713D329ECD}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>K K:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Mock Interview Prepartion</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="D3" authorId="0" shapeId="0" xr:uid="{0A17E92C-6FF0-4A33-A645-E6D149F8902C}">
       <text>
         <r>
@@ -429,6 +478,30 @@
           </rPr>
           <t xml:space="preserve">
 Health Issue</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AB5" authorId="2" shapeId="0" xr:uid="{2C5FC359-948E-4865-A650-F0A97C5C6A1F}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>K K:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Medical Emergency</t>
         </r>
       </text>
     </comment>
@@ -1008,6 +1081,226 @@
           </rPr>
           <t xml:space="preserve">
 Eye Operation</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AB9" authorId="2" shapeId="0" xr:uid="{1497B6CD-6E4B-40F4-A672-3B84F52DA68A}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>K K:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Eye Operation</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AC9" authorId="2" shapeId="0" xr:uid="{DEBB27FC-203D-480E-A933-18990BC5C2B0}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>K K:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Eye Operation</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AD9" authorId="2" shapeId="0" xr:uid="{C07B2C36-236F-414B-B79C-0916B7B2D883}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>K K:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Eye Operation</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AE9" authorId="2" shapeId="0" xr:uid="{7FA4D234-0D14-4ECC-B506-255AA1A2080F}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>K K:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Eye Operation</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>K K</author>
+  </authors>
+  <commentList>
+    <comment ref="F2" authorId="0" shapeId="0" xr:uid="{4122427C-8662-4349-A902-63C1477CDFF7}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>K K:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Going Outside</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H2" authorId="0" shapeId="0" xr:uid="{E38DA15E-0ED9-47CE-B2C5-D3F9C542B693}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Helath is not well</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I2" authorId="0" shapeId="0" xr:uid="{E9E8A71D-EB37-4D71-B771-5E88DA6CD438}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Helath is not well</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D3" authorId="0" shapeId="0" xr:uid="{3F09A33B-C66C-4DDE-ACA8-30103850DDB2}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>K K:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Family Function</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E3" authorId="0" shapeId="0" xr:uid="{80391759-E892-4D95-9DDC-676328C6B794}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>K K:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Out of Town</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H5" authorId="0" shapeId="0" xr:uid="{5ABEAE49-8EB0-4F4D-B753-09D032F88971}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Helath is not well</t>
         </r>
       </text>
     </comment>
@@ -1016,7 +1309,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="20">
   <si>
     <t>Student Name</t>
   </si>
@@ -1532,10 +1825,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF336CF2-9F7E-9D47-A242-C3CB362C49F8}">
-  <dimension ref="A1:AL19"/>
+  <dimension ref="A1:AK19"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="AC5" sqref="AC5"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1545,7 +1838,7 @@
     <col min="4" max="4" width="11.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:37" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -1627,8 +1920,20 @@
       <c r="AA1" s="4">
         <v>45317</v>
       </c>
+      <c r="AB1" s="4">
+        <v>45318</v>
+      </c>
+      <c r="AC1" s="4">
+        <v>45320</v>
+      </c>
+      <c r="AD1" s="4">
+        <v>45321</v>
+      </c>
+      <c r="AE1" s="4">
+        <v>45322</v>
+      </c>
     </row>
-    <row r="2" spans="1:38" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:37" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -1710,19 +2015,26 @@
       <c r="AA2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="AB2" s="6"/>
-      <c r="AC2" s="6"/>
-      <c r="AD2" s="6"/>
-      <c r="AE2" s="6"/>
+      <c r="AB2" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="AC2" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="AD2" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="AE2" s="6" t="s">
+        <v>11</v>
+      </c>
       <c r="AF2" s="6"/>
       <c r="AG2" s="6"/>
       <c r="AH2" s="6"/>
       <c r="AI2" s="6"/>
       <c r="AJ2" s="6"/>
       <c r="AK2" s="6"/>
-      <c r="AL2" s="6"/>
     </row>
-    <row r="3" spans="1:38" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:37" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="5">
         <v>2</v>
       </c>
@@ -1804,19 +2116,26 @@
       <c r="AA3" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="AB3" s="6"/>
-      <c r="AC3" s="6"/>
-      <c r="AD3" s="6"/>
-      <c r="AE3" s="6"/>
+      <c r="AB3" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="AC3" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="AD3" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="AE3" s="6" t="s">
+        <v>2</v>
+      </c>
       <c r="AF3" s="6"/>
       <c r="AG3" s="6"/>
       <c r="AH3" s="6"/>
       <c r="AI3" s="6"/>
       <c r="AJ3" s="6"/>
       <c r="AK3" s="6"/>
-      <c r="AL3" s="6"/>
     </row>
-    <row r="4" spans="1:38" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:37" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A4" s="5">
         <v>3</v>
       </c>
@@ -1898,19 +2217,26 @@
       <c r="AA4" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="AB4" s="6"/>
-      <c r="AC4" s="6"/>
-      <c r="AD4" s="6"/>
-      <c r="AE4" s="6"/>
+      <c r="AB4" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="AC4" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="AD4" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="AE4" s="6" t="s">
+        <v>2</v>
+      </c>
       <c r="AF4" s="6"/>
       <c r="AG4" s="6"/>
       <c r="AH4" s="6"/>
       <c r="AI4" s="6"/>
       <c r="AJ4" s="6"/>
       <c r="AK4" s="6"/>
-      <c r="AL4" s="6"/>
     </row>
-    <row r="5" spans="1:38" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:37" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A5" s="5">
         <v>4</v>
       </c>
@@ -1992,19 +2318,26 @@
       <c r="AA5" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="AB5" s="6"/>
-      <c r="AC5" s="6"/>
-      <c r="AD5" s="6"/>
-      <c r="AE5" s="6"/>
+      <c r="AB5" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="AC5" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="AD5" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="AE5" s="6" t="s">
+        <v>2</v>
+      </c>
       <c r="AF5" s="6"/>
       <c r="AG5" s="6"/>
       <c r="AH5" s="6"/>
       <c r="AI5" s="6"/>
       <c r="AJ5" s="6"/>
       <c r="AK5" s="6"/>
-      <c r="AL5" s="6"/>
     </row>
-    <row r="6" spans="1:38" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:37" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A6" s="5">
         <v>5</v>
       </c>
@@ -2086,19 +2419,26 @@
       <c r="AA6" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="AB6" s="6"/>
-      <c r="AC6" s="6"/>
-      <c r="AD6" s="6"/>
-      <c r="AE6" s="6"/>
+      <c r="AB6" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="AC6" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="AD6" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="AE6" s="6" t="s">
+        <v>2</v>
+      </c>
       <c r="AF6" s="6"/>
       <c r="AG6" s="6"/>
       <c r="AH6" s="6"/>
       <c r="AI6" s="6"/>
       <c r="AJ6" s="6"/>
       <c r="AK6" s="6"/>
-      <c r="AL6" s="6"/>
     </row>
-    <row r="7" spans="1:38" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:37" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A7" s="5">
         <v>6</v>
       </c>
@@ -2180,19 +2520,26 @@
       <c r="AA7" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="AB7" s="6"/>
-      <c r="AC7" s="6"/>
-      <c r="AD7" s="6"/>
-      <c r="AE7" s="6"/>
+      <c r="AB7" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC7" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD7" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="AE7" s="6" t="s">
+        <v>13</v>
+      </c>
       <c r="AF7" s="6"/>
       <c r="AG7" s="6"/>
       <c r="AH7" s="6"/>
       <c r="AI7" s="6"/>
       <c r="AJ7" s="6"/>
       <c r="AK7" s="6"/>
-      <c r="AL7" s="6"/>
     </row>
-    <row r="8" spans="1:38" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:37" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A8" s="5">
         <v>7</v>
       </c>
@@ -2274,19 +2621,26 @@
       <c r="AA8" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="AB8" s="6"/>
-      <c r="AC8" s="6"/>
-      <c r="AD8" s="6"/>
-      <c r="AE8" s="6"/>
+      <c r="AB8" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="AC8" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="AD8" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="AE8" s="6" t="s">
+        <v>2</v>
+      </c>
       <c r="AF8" s="6"/>
       <c r="AG8" s="6"/>
       <c r="AH8" s="6"/>
       <c r="AI8" s="6"/>
       <c r="AJ8" s="6"/>
       <c r="AK8" s="6"/>
-      <c r="AL8" s="6"/>
     </row>
-    <row r="9" spans="1:38" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:37" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A9" s="5">
         <v>8</v>
       </c>
@@ -2368,34 +2722,41 @@
       <c r="AA9" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="AB9" s="6"/>
-      <c r="AC9" s="6"/>
-      <c r="AD9" s="6"/>
-      <c r="AE9" s="6"/>
+      <c r="AB9" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="AC9" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="AD9" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="AE9" s="6" t="s">
+        <v>11</v>
+      </c>
       <c r="AF9" s="6"/>
       <c r="AG9" s="6"/>
       <c r="AH9" s="6"/>
       <c r="AI9" s="6"/>
       <c r="AJ9" s="6"/>
       <c r="AK9" s="6"/>
-      <c r="AL9" s="6"/>
     </row>
-    <row r="12" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:37" x14ac:dyDescent="0.25">
       <c r="B12" s="7" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:37" x14ac:dyDescent="0.25">
       <c r="B14" s="8" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:37" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:37" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
         <v>16</v>
       </c>
@@ -2417,7 +2778,7 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:AL9" xr:uid="{F036FACA-372A-8349-BD3D-950830E988A4}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:AK9" xr:uid="{F036FACA-372A-8349-BD3D-950830E988A4}">
       <formula1>"Present, Absent,Reason"</formula1>
     </dataValidation>
   </dataValidations>
@@ -2425,4 +2786,292 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7116870F-32D1-4C5F-8AB2-7A5DF8E85C37}">
+  <dimension ref="A1:I9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L22" sqref="L22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="6.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="44.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11"/>
+    <col min="4" max="9" width="11.125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="4">
+        <v>45323</v>
+      </c>
+      <c r="D1" s="4">
+        <v>45324</v>
+      </c>
+      <c r="E1" s="4">
+        <v>45325</v>
+      </c>
+      <c r="F1" s="4">
+        <v>45327</v>
+      </c>
+      <c r="G1" s="4">
+        <v>45328</v>
+      </c>
+      <c r="H1" s="4">
+        <v>45329</v>
+      </c>
+      <c r="I1" s="4">
+        <v>45330</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A2" s="5">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A3" s="5">
+        <v>2</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A4" s="5">
+        <v>3</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="I4" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A5" s="5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="I5" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A6" s="5">
+        <v>5</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="I6" s="6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A7" s="5">
+        <v>6</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="I7" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A8" s="5">
+        <v>7</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="I8" s="6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A9" s="5">
+        <v>8</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="I9" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:I9" xr:uid="{C9749C0A-5546-490D-970A-531EAC12EF0B}">
+      <formula1>"Present, Absent,Reason"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>